<commit_message>
centroids of 100km counties
</commit_message>
<xml_diff>
--- a/output_data/MDP_1980_2008_updated.xlsx
+++ b/output_data/MDP_1980_2008_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louzeyu/Desktop/ra_biodiversity/output_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889511F5-5548-7049-A554-82FB4B73FE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3420FE51-EA73-214F-B958-C1397B191BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="31140" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3757,8 +3757,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4058,10 +4059,13 @@
   <dimension ref="A1:Q311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="17" max="17" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4112,7 +4116,7 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1232</v>
       </c>
     </row>
@@ -4153,7 +4157,7 @@
       <c r="N2" t="s">
         <v>95</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>6075</v>
       </c>
     </row>
@@ -4191,7 +4195,7 @@
       <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="1">
         <v>12086</v>
       </c>
     </row>
@@ -4235,7 +4239,7 @@
       <c r="N4" t="s">
         <v>48</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="1">
         <v>12086</v>
       </c>
     </row>
@@ -4279,7 +4283,7 @@
       <c r="N5" t="s">
         <v>457</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="1">
         <v>17043</v>
       </c>
     </row>
@@ -4320,7 +4324,7 @@
       <c r="L6" t="s">
         <v>23</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="1">
         <v>25027</v>
       </c>
     </row>
@@ -4361,7 +4365,7 @@
       <c r="L7" t="s">
         <v>23</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="1">
         <v>45015</v>
       </c>
     </row>
@@ -4402,7 +4406,7 @@
       <c r="L8" t="s">
         <v>103</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="1">
         <v>45079</v>
       </c>
     </row>
@@ -4452,7 +4456,7 @@
       <c r="P9" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4502,7 +4506,7 @@
       <c r="P10" t="s">
         <v>50</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4549,7 +4553,7 @@
       <c r="P11" t="s">
         <v>26</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4596,7 +4600,7 @@
       <c r="P12" t="s">
         <v>84</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4643,7 +4647,7 @@
       <c r="P13" t="s">
         <v>84</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4690,7 +4694,7 @@
       <c r="P14" t="s">
         <v>74</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4737,7 +4741,7 @@
       <c r="P15" t="s">
         <v>74</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4781,7 +4785,7 @@
       <c r="P16" t="s">
         <v>41</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4831,7 +4835,7 @@
       <c r="P17" t="s">
         <v>67</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4881,7 +4885,7 @@
       <c r="P18" t="s">
         <v>58</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4928,7 +4932,7 @@
       <c r="P19" t="s">
         <v>105</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4975,7 +4979,7 @@
       <c r="P20" t="s">
         <v>105</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5025,7 +5029,7 @@
       <c r="P21" t="s">
         <v>97</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5072,7 +5076,7 @@
       <c r="P22" t="s">
         <v>137</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -5119,7 +5123,7 @@
       <c r="P23" t="s">
         <v>130</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="1" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5160,7 +5164,7 @@
       <c r="P24" t="s">
         <v>116</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -5207,7 +5211,7 @@
       <c r="P25" t="s">
         <v>123</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="1" t="s">
         <v>124</v>
       </c>
     </row>
@@ -5251,7 +5255,7 @@
       <c r="P26" t="s">
         <v>174</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="1" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5301,7 +5305,7 @@
       <c r="P27" t="s">
         <v>155</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q27" s="1" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5351,7 +5355,7 @@
       <c r="P28" t="s">
         <v>197</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="Q28" s="1" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5395,7 +5399,7 @@
       <c r="P29" t="s">
         <v>190</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="Q29" s="1" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5442,7 +5446,7 @@
       <c r="P30" t="s">
         <v>213</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="Q30" s="1" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5489,7 +5493,7 @@
       <c r="P31" t="s">
         <v>213</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q31" s="1" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5536,7 +5540,7 @@
       <c r="P32" t="s">
         <v>213</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="Q32" s="1" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5580,7 +5584,7 @@
       <c r="P33" t="s">
         <v>186</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="Q33" s="1" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5624,7 +5628,7 @@
       <c r="P34" t="s">
         <v>168</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="Q34" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5668,7 +5672,7 @@
       <c r="P35" t="s">
         <v>145</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35" s="1" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5718,7 +5722,7 @@
       <c r="P36" t="s">
         <v>145</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q36" s="1" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5762,7 +5766,7 @@
       <c r="P37" t="s">
         <v>160</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="1" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5806,7 +5810,7 @@
       <c r="P38" t="s">
         <v>181</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="Q38" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5856,7 +5860,7 @@
       <c r="P39" t="s">
         <v>181</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="Q39" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5906,7 +5910,7 @@
       <c r="P40" t="s">
         <v>238</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="Q40" s="1" t="s">
         <v>239</v>
       </c>
     </row>
@@ -5956,7 +5960,7 @@
       <c r="P41" t="s">
         <v>233</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="Q41" s="1" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6003,7 +6007,7 @@
       <c r="P42" t="s">
         <v>233</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="Q42" s="1" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6047,7 +6051,7 @@
       <c r="P43" t="s">
         <v>227</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="Q43" s="1" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6091,7 +6095,7 @@
       <c r="P44" t="s">
         <v>222</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="Q44" s="1" t="s">
         <v>223</v>
       </c>
     </row>
@@ -6141,7 +6145,7 @@
       <c r="P45" t="s">
         <v>246</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="Q45" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6191,7 +6195,7 @@
       <c r="P46" t="s">
         <v>246</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="Q46" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6241,7 +6245,7 @@
       <c r="P47" t="s">
         <v>256</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="Q47" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6288,7 +6292,7 @@
       <c r="P48" t="s">
         <v>261</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="Q48" s="1" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6338,7 +6342,7 @@
       <c r="P49" t="s">
         <v>282</v>
       </c>
-      <c r="Q49" t="s">
+      <c r="Q49" s="1" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6385,7 +6389,7 @@
       <c r="P50" t="s">
         <v>282</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="Q50" s="1" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6429,7 +6433,7 @@
       <c r="P51" t="s">
         <v>269</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="Q51" s="1" t="s">
         <v>270</v>
       </c>
     </row>
@@ -6470,7 +6474,7 @@
       <c r="P52" t="s">
         <v>286</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="Q52" s="1" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6520,7 +6524,7 @@
       <c r="P53" t="s">
         <v>286</v>
       </c>
-      <c r="Q53" t="s">
+      <c r="Q53" s="1" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6570,7 +6574,7 @@
       <c r="P54" t="s">
         <v>310</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="Q54" s="1" t="s">
         <v>311</v>
       </c>
     </row>
@@ -6614,7 +6618,7 @@
       <c r="P55" t="s">
         <v>291</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="Q55" s="1" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6664,7 +6668,7 @@
       <c r="P56" t="s">
         <v>291</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="Q56" s="1" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6714,7 +6718,7 @@
       <c r="P57" t="s">
         <v>291</v>
       </c>
-      <c r="Q57" t="s">
+      <c r="Q57" s="1" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6764,7 +6768,7 @@
       <c r="P58" t="s">
         <v>291</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="Q58" s="1" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6811,7 +6815,7 @@
       <c r="P59" t="s">
         <v>291</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="Q59" s="1" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6861,7 +6865,7 @@
       <c r="P60" t="s">
         <v>297</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="Q60" s="1" t="s">
         <v>298</v>
       </c>
     </row>
@@ -6905,7 +6909,7 @@
       <c r="P61" t="s">
         <v>274</v>
       </c>
-      <c r="Q61" t="s">
+      <c r="Q61" s="1" t="s">
         <v>275</v>
       </c>
     </row>
@@ -6955,7 +6959,7 @@
       <c r="P62" t="s">
         <v>315</v>
       </c>
-      <c r="Q62" t="s">
+      <c r="Q62" s="1" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7005,7 +7009,7 @@
       <c r="P63" t="s">
         <v>304</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="Q63" s="1" t="s">
         <v>305</v>
       </c>
     </row>
@@ -7055,7 +7059,7 @@
       <c r="P64" t="s">
         <v>377</v>
       </c>
-      <c r="Q64" t="s">
+      <c r="Q64" s="1" t="s">
         <v>378</v>
       </c>
     </row>
@@ -7105,7 +7109,7 @@
       <c r="P65" t="s">
         <v>411</v>
       </c>
-      <c r="Q65" t="s">
+      <c r="Q65" s="1" t="s">
         <v>412</v>
       </c>
     </row>
@@ -7155,7 +7159,7 @@
       <c r="P66" t="s">
         <v>404</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="Q66" s="1" t="s">
         <v>405</v>
       </c>
     </row>
@@ -7199,7 +7203,7 @@
       <c r="P67" t="s">
         <v>404</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="Q67" s="1" t="s">
         <v>405</v>
       </c>
     </row>
@@ -7246,7 +7250,7 @@
       <c r="P68" t="s">
         <v>415</v>
       </c>
-      <c r="Q68" t="s">
+      <c r="Q68" s="1" t="s">
         <v>416</v>
       </c>
     </row>
@@ -7296,7 +7300,7 @@
       <c r="P69" t="s">
         <v>358</v>
       </c>
-      <c r="Q69" t="s">
+      <c r="Q69" s="1" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7340,7 +7344,7 @@
       <c r="P70" t="s">
         <v>389</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="Q70" s="1" t="s">
         <v>390</v>
       </c>
     </row>
@@ -7390,7 +7394,7 @@
       <c r="P71" t="s">
         <v>389</v>
       </c>
-      <c r="Q71" t="s">
+      <c r="Q71" s="1" t="s">
         <v>390</v>
       </c>
     </row>
@@ -7440,7 +7444,7 @@
       <c r="P72" t="s">
         <v>389</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="Q72" s="1" t="s">
         <v>390</v>
       </c>
     </row>
@@ -7487,7 +7491,7 @@
       <c r="P73" t="s">
         <v>342</v>
       </c>
-      <c r="Q73" t="s">
+      <c r="Q73" s="1" t="s">
         <v>343</v>
       </c>
     </row>
@@ -7534,7 +7538,7 @@
       <c r="P74" t="s">
         <v>336</v>
       </c>
-      <c r="Q74" t="s">
+      <c r="Q74" s="1" t="s">
         <v>337</v>
       </c>
     </row>
@@ -7578,7 +7582,7 @@
       <c r="P75" t="s">
         <v>428</v>
       </c>
-      <c r="Q75" t="s">
+      <c r="Q75" s="1" t="s">
         <v>429</v>
       </c>
     </row>
@@ -7622,7 +7626,7 @@
       <c r="P76" t="s">
         <v>386</v>
       </c>
-      <c r="Q76" t="s">
+      <c r="Q76" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7672,7 +7676,7 @@
       <c r="P77" t="s">
         <v>386</v>
       </c>
-      <c r="Q77" t="s">
+      <c r="Q77" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7722,7 +7726,7 @@
       <c r="P78" t="s">
         <v>386</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="Q78" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7772,7 +7776,7 @@
       <c r="P79" t="s">
         <v>386</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="Q79" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7822,7 +7826,7 @@
       <c r="P80" t="s">
         <v>386</v>
       </c>
-      <c r="Q80" t="s">
+      <c r="Q80" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7872,7 +7876,7 @@
       <c r="P81" t="s">
         <v>386</v>
       </c>
-      <c r="Q81" t="s">
+      <c r="Q81" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7922,7 +7926,7 @@
       <c r="P82" t="s">
         <v>386</v>
       </c>
-      <c r="Q82" t="s">
+      <c r="Q82" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7969,7 +7973,7 @@
       <c r="P83" t="s">
         <v>386</v>
       </c>
-      <c r="Q83" t="s">
+      <c r="Q83" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -8016,7 +8020,7 @@
       <c r="P84" t="s">
         <v>395</v>
       </c>
-      <c r="Q84" t="s">
+      <c r="Q84" s="1" t="s">
         <v>396</v>
       </c>
     </row>
@@ -8060,7 +8064,7 @@
       <c r="P85" t="s">
         <v>382</v>
       </c>
-      <c r="Q85" t="s">
+      <c r="Q85" s="1" t="s">
         <v>383</v>
       </c>
     </row>
@@ -8110,7 +8114,7 @@
       <c r="P86" t="s">
         <v>423</v>
       </c>
-      <c r="Q86" t="s">
+      <c r="Q86" s="1" t="s">
         <v>424</v>
       </c>
     </row>
@@ -8157,7 +8161,7 @@
       <c r="P87" t="s">
         <v>350</v>
       </c>
-      <c r="Q87" t="s">
+      <c r="Q87" s="1" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8201,7 +8205,7 @@
       <c r="P88" t="s">
         <v>368</v>
       </c>
-      <c r="Q88" t="s">
+      <c r="Q88" s="1" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8245,7 +8249,7 @@
       <c r="P89" t="s">
         <v>363</v>
       </c>
-      <c r="Q89" t="s">
+      <c r="Q89" s="1" t="s">
         <v>364</v>
       </c>
     </row>
@@ -8295,7 +8299,7 @@
       <c r="P90" t="s">
         <v>450</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="Q90" s="1" t="s">
         <v>451</v>
       </c>
     </row>
@@ -8339,7 +8343,7 @@
       <c r="P91" t="s">
         <v>446</v>
       </c>
-      <c r="Q91" t="s">
+      <c r="Q91" s="1" t="s">
         <v>447</v>
       </c>
     </row>
@@ -8383,7 +8387,7 @@
       <c r="P92" t="s">
         <v>440</v>
       </c>
-      <c r="Q92" t="s">
+      <c r="Q92" s="1" t="s">
         <v>441</v>
       </c>
     </row>
@@ -8424,7 +8428,7 @@
       <c r="P93" t="s">
         <v>436</v>
       </c>
-      <c r="Q93" t="s">
+      <c r="Q93" s="1" t="s">
         <v>437</v>
       </c>
     </row>
@@ -8474,7 +8478,7 @@
       <c r="P94" t="s">
         <v>505</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="Q94" s="1" t="s">
         <v>506</v>
       </c>
     </row>
@@ -8518,7 +8522,7 @@
       <c r="P95" t="s">
         <v>474</v>
       </c>
-      <c r="Q95" t="s">
+      <c r="Q95" s="1" t="s">
         <v>475</v>
       </c>
     </row>
@@ -8568,7 +8572,7 @@
       <c r="P96" t="s">
         <v>479</v>
       </c>
-      <c r="Q96" t="s">
+      <c r="Q96" s="1" t="s">
         <v>480</v>
       </c>
     </row>
@@ -8612,7 +8616,7 @@
       <c r="P97" t="s">
         <v>462</v>
       </c>
-      <c r="Q97" t="s">
+      <c r="Q97" s="1" t="s">
         <v>463</v>
       </c>
     </row>
@@ -8659,7 +8663,7 @@
       <c r="P98" t="s">
         <v>462</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="Q98" s="1" t="s">
         <v>463</v>
       </c>
     </row>
@@ -8709,7 +8713,7 @@
       <c r="P99" t="s">
         <v>488</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="Q99" s="1" t="s">
         <v>489</v>
       </c>
     </row>
@@ -8759,7 +8763,7 @@
       <c r="P100" t="s">
         <v>500</v>
       </c>
-      <c r="Q100" t="s">
+      <c r="Q100" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -8800,7 +8804,7 @@
       <c r="P101" t="s">
         <v>470</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="Q101" s="1" t="s">
         <v>471</v>
       </c>
     </row>
@@ -8841,7 +8845,7 @@
       <c r="P102" t="s">
         <v>467</v>
       </c>
-      <c r="Q102" t="s">
+      <c r="Q102" s="1" t="s">
         <v>468</v>
       </c>
     </row>
@@ -8891,7 +8895,7 @@
       <c r="P103" t="s">
         <v>467</v>
       </c>
-      <c r="Q103" t="s">
+      <c r="Q103" s="1" t="s">
         <v>468</v>
       </c>
     </row>
@@ -8941,7 +8945,7 @@
       <c r="P104" t="s">
         <v>513</v>
       </c>
-      <c r="Q104" t="s">
+      <c r="Q104" s="1" t="s">
         <v>514</v>
       </c>
     </row>
@@ -8988,7 +8992,7 @@
       <c r="P105" t="s">
         <v>520</v>
       </c>
-      <c r="Q105" t="s">
+      <c r="Q105" s="1" t="s">
         <v>521</v>
       </c>
     </row>
@@ -9038,7 +9042,7 @@
       <c r="P106" t="s">
         <v>542</v>
       </c>
-      <c r="Q106" t="s">
+      <c r="Q106" s="1" t="s">
         <v>543</v>
       </c>
     </row>
@@ -9082,7 +9086,7 @@
       <c r="P107" t="s">
         <v>531</v>
       </c>
-      <c r="Q107" t="s">
+      <c r="Q107" s="1" t="s">
         <v>532</v>
       </c>
     </row>
@@ -9126,7 +9130,7 @@
       <c r="P108" t="s">
         <v>535</v>
       </c>
-      <c r="Q108" t="s">
+      <c r="Q108" s="1" t="s">
         <v>536</v>
       </c>
     </row>
@@ -9167,7 +9171,7 @@
       <c r="P109" t="s">
         <v>526</v>
       </c>
-      <c r="Q109" t="s">
+      <c r="Q109" s="1" t="s">
         <v>527</v>
       </c>
     </row>
@@ -9214,7 +9218,7 @@
       <c r="P110" t="s">
         <v>583</v>
       </c>
-      <c r="Q110" t="s">
+      <c r="Q110" s="1" t="s">
         <v>584</v>
       </c>
     </row>
@@ -9261,7 +9265,7 @@
       <c r="P111" t="s">
         <v>550</v>
       </c>
-      <c r="Q111" t="s">
+      <c r="Q111" s="1" t="s">
         <v>551</v>
       </c>
     </row>
@@ -9308,7 +9312,7 @@
       <c r="P112" t="s">
         <v>571</v>
       </c>
-      <c r="Q112" t="s">
+      <c r="Q112" s="1" t="s">
         <v>572</v>
       </c>
     </row>
@@ -9358,7 +9362,7 @@
       <c r="P113" t="s">
         <v>565</v>
       </c>
-      <c r="Q113" t="s">
+      <c r="Q113" s="1" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9408,7 +9412,7 @@
       <c r="P114" t="s">
         <v>565</v>
       </c>
-      <c r="Q114" t="s">
+      <c r="Q114" s="1" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9458,7 +9462,7 @@
       <c r="P115" t="s">
         <v>565</v>
       </c>
-      <c r="Q115" t="s">
+      <c r="Q115" s="1" t="s">
         <v>566</v>
       </c>
     </row>
@@ -9505,7 +9509,7 @@
       <c r="P116" t="s">
         <v>577</v>
       </c>
-      <c r="Q116" t="s">
+      <c r="Q116" s="1" t="s">
         <v>578</v>
       </c>
     </row>
@@ -9549,7 +9553,7 @@
       <c r="P117" t="s">
         <v>554</v>
       </c>
-      <c r="Q117" t="s">
+      <c r="Q117" s="1" t="s">
         <v>555</v>
       </c>
     </row>
@@ -9593,7 +9597,7 @@
       <c r="P118" t="s">
         <v>562</v>
       </c>
-      <c r="Q118" t="s">
+      <c r="Q118" s="1" t="s">
         <v>563</v>
       </c>
     </row>
@@ -9640,7 +9644,7 @@
       <c r="P119" t="s">
         <v>562</v>
       </c>
-      <c r="Q119" t="s">
+      <c r="Q119" s="1" t="s">
         <v>563</v>
       </c>
     </row>
@@ -9684,7 +9688,7 @@
       <c r="P120" t="s">
         <v>558</v>
       </c>
-      <c r="Q120" t="s">
+      <c r="Q120" s="1" t="s">
         <v>559</v>
       </c>
     </row>
@@ -9725,7 +9729,7 @@
       <c r="P121" t="s">
         <v>594</v>
       </c>
-      <c r="Q121" t="s">
+      <c r="Q121" s="1" t="s">
         <v>595</v>
       </c>
     </row>
@@ -9769,7 +9773,7 @@
       <c r="P122" t="s">
         <v>591</v>
       </c>
-      <c r="Q122" t="s">
+      <c r="Q122" s="1" t="s">
         <v>592</v>
       </c>
     </row>
@@ -9816,7 +9820,7 @@
       <c r="P123" t="s">
         <v>601</v>
       </c>
-      <c r="Q123" t="s">
+      <c r="Q123" s="1" t="s">
         <v>602</v>
       </c>
     </row>
@@ -9860,7 +9864,7 @@
       <c r="P124" t="s">
         <v>608</v>
       </c>
-      <c r="Q124" t="s">
+      <c r="Q124" s="1" t="s">
         <v>609</v>
       </c>
     </row>
@@ -9907,7 +9911,7 @@
       <c r="P125" t="s">
         <v>605</v>
       </c>
-      <c r="Q125" t="s">
+      <c r="Q125" s="1" t="s">
         <v>606</v>
       </c>
     </row>
@@ -9957,7 +9961,7 @@
       <c r="P126" t="s">
         <v>617</v>
       </c>
-      <c r="Q126" t="s">
+      <c r="Q126" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -9998,7 +10002,7 @@
       <c r="P127" t="s">
         <v>621</v>
       </c>
-      <c r="Q127" t="s">
+      <c r="Q127" s="1" t="s">
         <v>622</v>
       </c>
     </row>
@@ -10048,7 +10052,7 @@
       <c r="P128" t="s">
         <v>628</v>
       </c>
-      <c r="Q128" t="s">
+      <c r="Q128" s="1" t="s">
         <v>629</v>
       </c>
     </row>
@@ -10098,7 +10102,7 @@
       <c r="P129" t="s">
         <v>646</v>
       </c>
-      <c r="Q129" t="s">
+      <c r="Q129" s="1" t="s">
         <v>647</v>
       </c>
     </row>
@@ -10148,7 +10152,7 @@
       <c r="P130" t="s">
         <v>642</v>
       </c>
-      <c r="Q130" t="s">
+      <c r="Q130" s="1" t="s">
         <v>643</v>
       </c>
     </row>
@@ -10198,7 +10202,7 @@
       <c r="P131" t="s">
         <v>642</v>
       </c>
-      <c r="Q131" t="s">
+      <c r="Q131" s="1" t="s">
         <v>643</v>
       </c>
     </row>
@@ -10242,7 +10246,7 @@
       <c r="P132" t="s">
         <v>636</v>
       </c>
-      <c r="Q132" t="s">
+      <c r="Q132" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -10286,7 +10290,7 @@
       <c r="P133" t="s">
         <v>654</v>
       </c>
-      <c r="Q133" t="s">
+      <c r="Q133" s="1" t="s">
         <v>655</v>
       </c>
     </row>
@@ -10333,7 +10337,7 @@
       <c r="P134" t="s">
         <v>654</v>
       </c>
-      <c r="Q134" t="s">
+      <c r="Q134" s="1" t="s">
         <v>655</v>
       </c>
     </row>
@@ -10380,7 +10384,7 @@
       <c r="P135" t="s">
         <v>669</v>
       </c>
-      <c r="Q135" t="s">
+      <c r="Q135" s="1" t="s">
         <v>670</v>
       </c>
     </row>
@@ -10427,7 +10431,7 @@
       <c r="P136" t="s">
         <v>661</v>
       </c>
-      <c r="Q136" t="s">
+      <c r="Q136" s="1" t="s">
         <v>662</v>
       </c>
     </row>
@@ -10477,7 +10481,7 @@
       <c r="P137" t="s">
         <v>665</v>
       </c>
-      <c r="Q137" t="s">
+      <c r="Q137" s="1" t="s">
         <v>666</v>
       </c>
     </row>
@@ -10527,7 +10531,7 @@
       <c r="P138" t="s">
         <v>682</v>
       </c>
-      <c r="Q138" t="s">
+      <c r="Q138" s="1" t="s">
         <v>683</v>
       </c>
     </row>
@@ -10577,7 +10581,7 @@
       <c r="P139" t="s">
         <v>678</v>
       </c>
-      <c r="Q139" t="s">
+      <c r="Q139" s="1" t="s">
         <v>679</v>
       </c>
     </row>
@@ -10627,7 +10631,7 @@
       <c r="P140" t="s">
         <v>688</v>
       </c>
-      <c r="Q140" t="s">
+      <c r="Q140" s="1" t="s">
         <v>689</v>
       </c>
     </row>
@@ -10674,7 +10678,7 @@
       <c r="P141" t="s">
         <v>688</v>
       </c>
-      <c r="Q141" t="s">
+      <c r="Q141" s="1" t="s">
         <v>689</v>
       </c>
     </row>
@@ -10721,7 +10725,7 @@
       <c r="P142" t="s">
         <v>696</v>
       </c>
-      <c r="Q142" t="s">
+      <c r="Q142" s="1" t="s">
         <v>697</v>
       </c>
     </row>
@@ -10768,7 +10772,7 @@
       <c r="P143" t="s">
         <v>693</v>
       </c>
-      <c r="Q143" t="s">
+      <c r="Q143" s="1" t="s">
         <v>694</v>
       </c>
     </row>
@@ -10818,7 +10822,7 @@
       <c r="P144" t="s">
         <v>721</v>
       </c>
-      <c r="Q144" t="s">
+      <c r="Q144" s="1" t="s">
         <v>722</v>
       </c>
     </row>
@@ -10868,7 +10872,7 @@
       <c r="P145" t="s">
         <v>718</v>
       </c>
-      <c r="Q145" t="s">
+      <c r="Q145" s="1" t="s">
         <v>719</v>
       </c>
     </row>
@@ -10918,7 +10922,7 @@
       <c r="P146" t="s">
         <v>715</v>
       </c>
-      <c r="Q146" t="s">
+      <c r="Q146" s="1" t="s">
         <v>716</v>
       </c>
     </row>
@@ -10968,7 +10972,7 @@
       <c r="P147" t="s">
         <v>725</v>
       </c>
-      <c r="Q147" t="s">
+      <c r="Q147" s="1" t="s">
         <v>726</v>
       </c>
     </row>
@@ -11009,7 +11013,7 @@
       <c r="P148" t="s">
         <v>704</v>
       </c>
-      <c r="Q148" t="s">
+      <c r="Q148" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -11050,7 +11054,7 @@
       <c r="P149" t="s">
         <v>708</v>
       </c>
-      <c r="Q149" t="s">
+      <c r="Q149" s="1" t="s">
         <v>709</v>
       </c>
     </row>
@@ -11100,7 +11104,7 @@
       <c r="P150" t="s">
         <v>708</v>
       </c>
-      <c r="Q150" t="s">
+      <c r="Q150" s="1" t="s">
         <v>709</v>
       </c>
     </row>
@@ -11147,7 +11151,7 @@
       <c r="P151" t="s">
         <v>708</v>
       </c>
-      <c r="Q151" t="s">
+      <c r="Q151" s="1" t="s">
         <v>709</v>
       </c>
     </row>
@@ -11188,7 +11192,7 @@
       <c r="P152" t="s">
         <v>711</v>
       </c>
-      <c r="Q152" t="s">
+      <c r="Q152" s="1" t="s">
         <v>712</v>
       </c>
     </row>
@@ -11238,7 +11242,7 @@
       <c r="P153" t="s">
         <v>711</v>
       </c>
-      <c r="Q153" t="s">
+      <c r="Q153" s="1" t="s">
         <v>712</v>
       </c>
     </row>
@@ -11285,7 +11289,7 @@
       <c r="P154" t="s">
         <v>711</v>
       </c>
-      <c r="Q154" t="s">
+      <c r="Q154" s="1" t="s">
         <v>712</v>
       </c>
     </row>
@@ -11335,7 +11339,7 @@
       <c r="P155" t="s">
         <v>733</v>
       </c>
-      <c r="Q155" t="s">
+      <c r="Q155" s="1" t="s">
         <v>734</v>
       </c>
     </row>
@@ -11382,7 +11386,7 @@
       <c r="P156" t="s">
         <v>733</v>
       </c>
-      <c r="Q156" t="s">
+      <c r="Q156" s="1" t="s">
         <v>734</v>
       </c>
     </row>
@@ -11432,7 +11436,7 @@
       <c r="P157" t="s">
         <v>733</v>
       </c>
-      <c r="Q157" t="s">
+      <c r="Q157" s="1" t="s">
         <v>734</v>
       </c>
     </row>
@@ -11482,7 +11486,7 @@
       <c r="P158" t="s">
         <v>733</v>
       </c>
-      <c r="Q158" t="s">
+      <c r="Q158" s="1" t="s">
         <v>734</v>
       </c>
     </row>
@@ -11532,7 +11536,7 @@
       <c r="P159" t="s">
         <v>743</v>
       </c>
-      <c r="Q159" t="s">
+      <c r="Q159" s="1" t="s">
         <v>744</v>
       </c>
     </row>
@@ -11576,7 +11580,7 @@
       <c r="P160" t="s">
         <v>750</v>
       </c>
-      <c r="Q160" t="s">
+      <c r="Q160" s="1" t="s">
         <v>751</v>
       </c>
     </row>
@@ -11626,7 +11630,7 @@
       <c r="P161" t="s">
         <v>750</v>
       </c>
-      <c r="Q161" t="s">
+      <c r="Q161" s="1" t="s">
         <v>751</v>
       </c>
     </row>
@@ -11667,7 +11671,7 @@
       <c r="P162" t="s">
         <v>756</v>
       </c>
-      <c r="Q162" t="s">
+      <c r="Q162" s="1" t="s">
         <v>757</v>
       </c>
     </row>
@@ -11717,7 +11721,7 @@
       <c r="P163" t="s">
         <v>763</v>
       </c>
-      <c r="Q163" t="s">
+      <c r="Q163" s="1" t="s">
         <v>764</v>
       </c>
     </row>
@@ -11758,7 +11762,7 @@
       <c r="P164" t="s">
         <v>759</v>
       </c>
-      <c r="Q164" t="s">
+      <c r="Q164" s="1" t="s">
         <v>760</v>
       </c>
     </row>
@@ -11808,7 +11812,7 @@
       <c r="P165" t="s">
         <v>759</v>
       </c>
-      <c r="Q165" t="s">
+      <c r="Q165" s="1" t="s">
         <v>760</v>
       </c>
     </row>
@@ -11858,7 +11862,7 @@
       <c r="P166" t="s">
         <v>777</v>
       </c>
-      <c r="Q166" t="s">
+      <c r="Q166" s="1" t="s">
         <v>778</v>
       </c>
     </row>
@@ -11908,7 +11912,7 @@
       <c r="P167" t="s">
         <v>769</v>
       </c>
-      <c r="Q167" t="s">
+      <c r="Q167" s="1" t="s">
         <v>770</v>
       </c>
     </row>
@@ -11952,7 +11956,7 @@
       <c r="P168" t="s">
         <v>783</v>
       </c>
-      <c r="Q168" t="s">
+      <c r="Q168" s="1" t="s">
         <v>784</v>
       </c>
     </row>
@@ -11996,7 +12000,7 @@
       <c r="P169" t="s">
         <v>783</v>
       </c>
-      <c r="Q169" t="s">
+      <c r="Q169" s="1" t="s">
         <v>784</v>
       </c>
     </row>
@@ -12043,7 +12047,7 @@
       <c r="P170" t="s">
         <v>842</v>
       </c>
-      <c r="Q170" t="s">
+      <c r="Q170" s="1" t="s">
         <v>843</v>
       </c>
     </row>
@@ -12093,7 +12097,7 @@
       <c r="P171" t="s">
         <v>830</v>
       </c>
-      <c r="Q171" t="s">
+      <c r="Q171" s="1" t="s">
         <v>831</v>
       </c>
     </row>
@@ -12140,7 +12144,7 @@
       <c r="P172" t="s">
         <v>830</v>
       </c>
-      <c r="Q172" t="s">
+      <c r="Q172" s="1" t="s">
         <v>831</v>
       </c>
     </row>
@@ -12190,7 +12194,7 @@
       <c r="P173" t="s">
         <v>815</v>
       </c>
-      <c r="Q173" t="s">
+      <c r="Q173" s="1" t="s">
         <v>816</v>
       </c>
     </row>
@@ -12240,7 +12244,7 @@
       <c r="P174" t="s">
         <v>823</v>
       </c>
-      <c r="Q174" t="s">
+      <c r="Q174" s="1" t="s">
         <v>824</v>
       </c>
     </row>
@@ -12287,7 +12291,7 @@
       <c r="P175" t="s">
         <v>823</v>
       </c>
-      <c r="Q175" t="s">
+      <c r="Q175" s="1" t="s">
         <v>824</v>
       </c>
     </row>
@@ -12334,7 +12338,7 @@
       <c r="P176" t="s">
         <v>846</v>
       </c>
-      <c r="Q176" t="s">
+      <c r="Q176" s="1" t="s">
         <v>847</v>
       </c>
     </row>
@@ -12381,7 +12385,7 @@
       <c r="P177" t="s">
         <v>836</v>
       </c>
-      <c r="Q177" t="s">
+      <c r="Q177" s="1" t="s">
         <v>837</v>
       </c>
     </row>
@@ -12431,7 +12435,7 @@
       <c r="P178" t="s">
         <v>811</v>
       </c>
-      <c r="Q178" t="s">
+      <c r="Q178" s="1" t="s">
         <v>812</v>
       </c>
     </row>
@@ -12481,7 +12485,7 @@
       <c r="P179" t="s">
         <v>819</v>
       </c>
-      <c r="Q179" t="s">
+      <c r="Q179" s="1" t="s">
         <v>820</v>
       </c>
     </row>
@@ -12531,7 +12535,7 @@
       <c r="P180" t="s">
         <v>796</v>
       </c>
-      <c r="Q180" t="s">
+      <c r="Q180" s="1" t="s">
         <v>797</v>
       </c>
     </row>
@@ -12575,7 +12579,7 @@
       <c r="P181" t="s">
         <v>796</v>
       </c>
-      <c r="Q181" t="s">
+      <c r="Q181" s="1" t="s">
         <v>797</v>
       </c>
     </row>
@@ -12622,7 +12626,7 @@
       <c r="P182" t="s">
         <v>789</v>
       </c>
-      <c r="Q182" t="s">
+      <c r="Q182" s="1" t="s">
         <v>790</v>
       </c>
     </row>
@@ -12669,7 +12673,7 @@
       <c r="P183" t="s">
         <v>833</v>
       </c>
-      <c r="Q183" t="s">
+      <c r="Q183" s="1" t="s">
         <v>834</v>
       </c>
     </row>
@@ -12719,7 +12723,7 @@
       <c r="P184" t="s">
         <v>802</v>
       </c>
-      <c r="Q184" t="s">
+      <c r="Q184" s="1" t="s">
         <v>803</v>
       </c>
     </row>
@@ -12769,7 +12773,7 @@
       <c r="P185" t="s">
         <v>873</v>
       </c>
-      <c r="Q185" t="s">
+      <c r="Q185" s="1" t="s">
         <v>874</v>
       </c>
     </row>
@@ -12813,7 +12817,7 @@
       <c r="P186" t="s">
         <v>863</v>
       </c>
-      <c r="Q186" t="s">
+      <c r="Q186" s="1" t="s">
         <v>864</v>
       </c>
     </row>
@@ -12857,7 +12861,7 @@
       <c r="P187" t="s">
         <v>898</v>
       </c>
-      <c r="Q187" t="s">
+      <c r="Q187" s="1" t="s">
         <v>899</v>
       </c>
     </row>
@@ -12904,7 +12908,7 @@
       <c r="P188" t="s">
         <v>893</v>
       </c>
-      <c r="Q188" t="s">
+      <c r="Q188" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -12954,7 +12958,7 @@
       <c r="P189" t="s">
         <v>868</v>
       </c>
-      <c r="Q189" t="s">
+      <c r="Q189" s="1" t="s">
         <v>869</v>
       </c>
     </row>
@@ -13001,7 +13005,7 @@
       <c r="P190" t="s">
         <v>868</v>
       </c>
-      <c r="Q190" t="s">
+      <c r="Q190" s="1" t="s">
         <v>869</v>
       </c>
     </row>
@@ -13051,7 +13055,7 @@
       <c r="P191" t="s">
         <v>883</v>
       </c>
-      <c r="Q191" t="s">
+      <c r="Q191" s="1" t="s">
         <v>884</v>
       </c>
     </row>
@@ -13098,7 +13102,7 @@
       <c r="P192" t="s">
         <v>889</v>
       </c>
-      <c r="Q192" t="s">
+      <c r="Q192" s="1" t="s">
         <v>890</v>
       </c>
     </row>
@@ -13145,7 +13149,7 @@
       <c r="P193" t="s">
         <v>855</v>
       </c>
-      <c r="Q193" t="s">
+      <c r="Q193" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13195,7 +13199,7 @@
       <c r="P194" t="s">
         <v>855</v>
       </c>
-      <c r="Q194" t="s">
+      <c r="Q194" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13245,7 +13249,7 @@
       <c r="P195" t="s">
         <v>855</v>
       </c>
-      <c r="Q195" t="s">
+      <c r="Q195" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13292,7 +13296,7 @@
       <c r="P196" t="s">
         <v>855</v>
       </c>
-      <c r="Q196" t="s">
+      <c r="Q196" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13339,7 +13343,7 @@
       <c r="P197" t="s">
         <v>855</v>
       </c>
-      <c r="Q197" t="s">
+      <c r="Q197" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13386,7 +13390,7 @@
       <c r="P198" t="s">
         <v>855</v>
       </c>
-      <c r="Q198" t="s">
+      <c r="Q198" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -13436,7 +13440,7 @@
       <c r="P199" t="s">
         <v>880</v>
       </c>
-      <c r="Q199" t="s">
+      <c r="Q199" s="1" t="s">
         <v>881</v>
       </c>
     </row>
@@ -13480,7 +13484,7 @@
       <c r="P200" t="s">
         <v>859</v>
       </c>
-      <c r="Q200" t="s">
+      <c r="Q200" s="1" t="s">
         <v>860</v>
       </c>
     </row>
@@ -13527,7 +13531,7 @@
       <c r="P201" t="s">
         <v>903</v>
       </c>
-      <c r="Q201" t="s">
+      <c r="Q201" s="1" t="s">
         <v>904</v>
       </c>
     </row>
@@ -13577,7 +13581,7 @@
       <c r="P202" t="s">
         <v>922</v>
       </c>
-      <c r="Q202" t="s">
+      <c r="Q202" s="1" t="s">
         <v>923</v>
       </c>
     </row>
@@ -13627,7 +13631,7 @@
       <c r="P203" t="s">
         <v>928</v>
       </c>
-      <c r="Q203" t="s">
+      <c r="Q203" s="1" t="s">
         <v>929</v>
       </c>
     </row>
@@ -13677,7 +13681,7 @@
       <c r="P204" t="s">
         <v>930</v>
       </c>
-      <c r="Q204" t="s">
+      <c r="Q204" s="1" t="s">
         <v>931</v>
       </c>
     </row>
@@ -13727,7 +13731,7 @@
       <c r="P205" t="s">
         <v>933</v>
       </c>
-      <c r="Q205" t="s">
+      <c r="Q205" s="1" t="s">
         <v>934</v>
       </c>
     </row>
@@ -13771,7 +13775,7 @@
       <c r="P206" t="s">
         <v>914</v>
       </c>
-      <c r="Q206" t="s">
+      <c r="Q206" s="1" t="s">
         <v>915</v>
       </c>
     </row>
@@ -13818,7 +13822,7 @@
       <c r="P207" t="s">
         <v>938</v>
       </c>
-      <c r="Q207" t="s">
+      <c r="Q207" s="1" t="s">
         <v>939</v>
       </c>
     </row>
@@ -13868,7 +13872,7 @@
       <c r="P208" t="s">
         <v>911</v>
       </c>
-      <c r="Q208" t="s">
+      <c r="Q208" s="1" t="s">
         <v>912</v>
       </c>
     </row>
@@ -13918,7 +13922,7 @@
       <c r="P209" t="s">
         <v>918</v>
       </c>
-      <c r="Q209" t="s">
+      <c r="Q209" s="1" t="s">
         <v>919</v>
       </c>
     </row>
@@ -13968,7 +13972,7 @@
       <c r="P210" t="s">
         <v>925</v>
       </c>
-      <c r="Q210" t="s">
+      <c r="Q210" s="1" t="s">
         <v>926</v>
       </c>
     </row>
@@ -14015,7 +14019,7 @@
       <c r="P211" t="s">
         <v>951</v>
       </c>
-      <c r="Q211" t="s">
+      <c r="Q211" s="1" t="s">
         <v>952</v>
       </c>
     </row>
@@ -14056,7 +14060,7 @@
       <c r="P212" t="s">
         <v>943</v>
       </c>
-      <c r="Q212" t="s">
+      <c r="Q212" s="1" t="s">
         <v>944</v>
       </c>
     </row>
@@ -14097,7 +14101,7 @@
       <c r="P213" t="s">
         <v>946</v>
       </c>
-      <c r="Q213" t="s">
+      <c r="Q213" s="1" t="s">
         <v>947</v>
       </c>
     </row>
@@ -14147,7 +14151,7 @@
       <c r="P214" t="s">
         <v>946</v>
       </c>
-      <c r="Q214" t="s">
+      <c r="Q214" s="1" t="s">
         <v>947</v>
       </c>
     </row>
@@ -14197,7 +14201,7 @@
       <c r="P215" t="s">
         <v>946</v>
       </c>
-      <c r="Q215" t="s">
+      <c r="Q215" s="1" t="s">
         <v>947</v>
       </c>
     </row>
@@ -14238,7 +14242,7 @@
       <c r="P216" t="s">
         <v>958</v>
       </c>
-      <c r="Q216" t="s">
+      <c r="Q216" s="1" t="s">
         <v>959</v>
       </c>
     </row>
@@ -14288,7 +14292,7 @@
       <c r="P217" t="s">
         <v>958</v>
       </c>
-      <c r="Q217" t="s">
+      <c r="Q217" s="1" t="s">
         <v>959</v>
       </c>
     </row>
@@ -14329,7 +14333,7 @@
       <c r="P218" t="s">
         <v>960</v>
       </c>
-      <c r="Q218" t="s">
+      <c r="Q218" s="1" t="s">
         <v>961</v>
       </c>
     </row>
@@ -14379,7 +14383,7 @@
       <c r="P219" t="s">
         <v>980</v>
       </c>
-      <c r="Q219" t="s">
+      <c r="Q219" s="1" t="s">
         <v>981</v>
       </c>
     </row>
@@ -14426,7 +14430,7 @@
       <c r="P220" t="s">
         <v>987</v>
       </c>
-      <c r="Q220" t="s">
+      <c r="Q220" s="1" t="s">
         <v>988</v>
       </c>
     </row>
@@ -14473,7 +14477,7 @@
       <c r="P221" t="s">
         <v>991</v>
       </c>
-      <c r="Q221" t="s">
+      <c r="Q221" s="1" t="s">
         <v>992</v>
       </c>
     </row>
@@ -14520,7 +14524,7 @@
       <c r="P222" t="s">
         <v>995</v>
       </c>
-      <c r="Q222" t="s">
+      <c r="Q222" s="1" t="s">
         <v>996</v>
       </c>
     </row>
@@ -14570,7 +14574,7 @@
       <c r="P223" t="s">
         <v>976</v>
       </c>
-      <c r="Q223" t="s">
+      <c r="Q223" s="1" t="s">
         <v>977</v>
       </c>
     </row>
@@ -14620,7 +14624,7 @@
       <c r="P224" t="s">
         <v>984</v>
       </c>
-      <c r="Q224" t="s">
+      <c r="Q224" s="1" t="s">
         <v>985</v>
       </c>
     </row>
@@ -14664,7 +14668,7 @@
       <c r="P225" t="s">
         <v>969</v>
       </c>
-      <c r="Q225" t="s">
+      <c r="Q225" s="1" t="s">
         <v>970</v>
       </c>
     </row>
@@ -14714,7 +14718,7 @@
       <c r="P226" t="s">
         <v>969</v>
       </c>
-      <c r="Q226" t="s">
+      <c r="Q226" s="1" t="s">
         <v>970</v>
       </c>
     </row>
@@ -14764,7 +14768,7 @@
       <c r="P227" t="s">
         <v>974</v>
       </c>
-      <c r="Q227" t="s">
+      <c r="Q227" s="1" t="s">
         <v>975</v>
       </c>
     </row>
@@ -14808,7 +14812,7 @@
       <c r="P228" t="s">
         <v>974</v>
       </c>
-      <c r="Q228" t="s">
+      <c r="Q228" s="1" t="s">
         <v>975</v>
       </c>
     </row>
@@ -14855,7 +14859,7 @@
       <c r="P229" t="s">
         <v>1024</v>
       </c>
-      <c r="Q229" t="s">
+      <c r="Q229" s="1" t="s">
         <v>1025</v>
       </c>
     </row>
@@ -14905,7 +14909,7 @@
       <c r="P230" t="s">
         <v>1004</v>
       </c>
-      <c r="Q230" t="s">
+      <c r="Q230" s="1" t="s">
         <v>1005</v>
       </c>
     </row>
@@ -14955,7 +14959,7 @@
       <c r="P231" t="s">
         <v>1022</v>
       </c>
-      <c r="Q231" t="s">
+      <c r="Q231" s="1" t="s">
         <v>1023</v>
       </c>
     </row>
@@ -14999,7 +15003,7 @@
       <c r="P232" t="s">
         <v>1000</v>
       </c>
-      <c r="Q232" t="s">
+      <c r="Q232" s="1" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -15049,7 +15053,7 @@
       <c r="P233" t="s">
         <v>1012</v>
       </c>
-      <c r="Q233" t="s">
+      <c r="Q233" s="1" t="s">
         <v>1013</v>
       </c>
     </row>
@@ -15093,7 +15097,7 @@
       <c r="P234" t="s">
         <v>1007</v>
       </c>
-      <c r="Q234" t="s">
+      <c r="Q234" s="1" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -15137,7 +15141,7 @@
       <c r="P235" t="s">
         <v>1007</v>
       </c>
-      <c r="Q235" t="s">
+      <c r="Q235" s="1" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -15187,7 +15191,7 @@
       <c r="P236" t="s">
         <v>1016</v>
       </c>
-      <c r="Q236" t="s">
+      <c r="Q236" s="1" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -15237,7 +15241,7 @@
       <c r="P237" t="s">
         <v>1016</v>
       </c>
-      <c r="Q237" t="s">
+      <c r="Q237" s="1" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -15284,7 +15288,7 @@
       <c r="P238" t="s">
         <v>1027</v>
       </c>
-      <c r="Q238" t="s">
+      <c r="Q238" s="1" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -15331,7 +15335,7 @@
       <c r="P239" t="s">
         <v>1070</v>
       </c>
-      <c r="Q239" t="s">
+      <c r="Q239" s="1" t="s">
         <v>1071</v>
       </c>
     </row>
@@ -15378,7 +15382,7 @@
       <c r="P240" t="s">
         <v>1036</v>
       </c>
-      <c r="Q240" t="s">
+      <c r="Q240" s="1" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -15425,7 +15429,7 @@
       <c r="P241" t="s">
         <v>1074</v>
       </c>
-      <c r="Q241" t="s">
+      <c r="Q241" s="1" t="s">
         <v>1075</v>
       </c>
     </row>
@@ -15472,7 +15476,7 @@
       <c r="P242" t="s">
         <v>1074</v>
       </c>
-      <c r="Q242" t="s">
+      <c r="Q242" s="1" t="s">
         <v>1075</v>
       </c>
     </row>
@@ -15516,7 +15520,7 @@
       <c r="P243" t="s">
         <v>1057</v>
       </c>
-      <c r="Q243" t="s">
+      <c r="Q243" s="1" t="s">
         <v>1058</v>
       </c>
     </row>
@@ -15566,7 +15570,7 @@
       <c r="P244" t="s">
         <v>1067</v>
       </c>
-      <c r="Q244" t="s">
+      <c r="Q244" s="1" t="s">
         <v>1068</v>
       </c>
     </row>
@@ -15616,7 +15620,7 @@
       <c r="P245" t="s">
         <v>1046</v>
       </c>
-      <c r="Q245" t="s">
+      <c r="Q245" s="1" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -15663,7 +15667,7 @@
       <c r="P246" t="s">
         <v>1077</v>
       </c>
-      <c r="Q246" t="s">
+      <c r="Q246" s="1" t="s">
         <v>1078</v>
       </c>
     </row>
@@ -15707,7 +15711,7 @@
       <c r="P247" t="s">
         <v>1041</v>
       </c>
-      <c r="Q247" t="s">
+      <c r="Q247" s="1" t="s">
         <v>1042</v>
       </c>
     </row>
@@ -15757,7 +15761,7 @@
       <c r="P248" t="s">
         <v>1063</v>
       </c>
-      <c r="Q248" t="s">
+      <c r="Q248" s="1" t="s">
         <v>1064</v>
       </c>
     </row>
@@ -15801,7 +15805,7 @@
       <c r="P249" t="s">
         <v>1060</v>
       </c>
-      <c r="Q249" t="s">
+      <c r="Q249" s="1" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -15845,7 +15849,7 @@
       <c r="P250" t="s">
         <v>1050</v>
       </c>
-      <c r="Q250" t="s">
+      <c r="Q250" s="1" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -15886,7 +15890,7 @@
       <c r="P251" t="s">
         <v>1053</v>
       </c>
-      <c r="Q251" t="s">
+      <c r="Q251" s="1" t="s">
         <v>1054</v>
       </c>
     </row>
@@ -15933,7 +15937,7 @@
       <c r="P252" t="s">
         <v>1141</v>
       </c>
-      <c r="Q252" t="s">
+      <c r="Q252" s="1" t="s">
         <v>1142</v>
       </c>
     </row>
@@ -15980,7 +15984,7 @@
       <c r="P253" t="s">
         <v>1137</v>
       </c>
-      <c r="Q253" t="s">
+      <c r="Q253" s="1" t="s">
         <v>1138</v>
       </c>
     </row>
@@ -16027,7 +16031,7 @@
       <c r="P254" t="s">
         <v>1106</v>
       </c>
-      <c r="Q254" t="s">
+      <c r="Q254" s="1" t="s">
         <v>1107</v>
       </c>
     </row>
@@ -16074,7 +16078,7 @@
       <c r="P255" t="s">
         <v>1101</v>
       </c>
-      <c r="Q255" t="s">
+      <c r="Q255" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16124,7 +16128,7 @@
       <c r="P256" t="s">
         <v>1101</v>
       </c>
-      <c r="Q256" t="s">
+      <c r="Q256" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16174,7 +16178,7 @@
       <c r="P257" t="s">
         <v>1101</v>
       </c>
-      <c r="Q257" t="s">
+      <c r="Q257" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16224,7 +16228,7 @@
       <c r="P258" t="s">
         <v>1101</v>
       </c>
-      <c r="Q258" t="s">
+      <c r="Q258" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16274,7 +16278,7 @@
       <c r="P259" t="s">
         <v>1101</v>
       </c>
-      <c r="Q259" t="s">
+      <c r="Q259" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16321,7 +16325,7 @@
       <c r="P260" t="s">
         <v>1101</v>
       </c>
-      <c r="Q260" t="s">
+      <c r="Q260" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16368,7 +16372,7 @@
       <c r="P261" t="s">
         <v>1101</v>
       </c>
-      <c r="Q261" t="s">
+      <c r="Q261" s="1" t="s">
         <v>1102</v>
       </c>
     </row>
@@ -16418,7 +16422,7 @@
       <c r="P262" t="s">
         <v>1121</v>
       </c>
-      <c r="Q262" t="s">
+      <c r="Q262" s="1" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -16462,7 +16466,7 @@
       <c r="P263" t="s">
         <v>1097</v>
       </c>
-      <c r="Q263" t="s">
+      <c r="Q263" s="1" t="s">
         <v>1098</v>
       </c>
     </row>
@@ -16512,7 +16516,7 @@
       <c r="P264" t="s">
         <v>1133</v>
       </c>
-      <c r="Q264" t="s">
+      <c r="Q264" s="1" t="s">
         <v>1134</v>
       </c>
     </row>
@@ -16556,7 +16560,7 @@
       <c r="P265" t="s">
         <v>1110</v>
       </c>
-      <c r="Q265" t="s">
+      <c r="Q265" s="1" t="s">
         <v>1111</v>
       </c>
     </row>
@@ -16600,7 +16604,7 @@
       <c r="P266" t="s">
         <v>1083</v>
       </c>
-      <c r="Q266" t="s">
+      <c r="Q266" s="1" t="s">
         <v>1084</v>
       </c>
     </row>
@@ -16644,7 +16648,7 @@
       <c r="P267" t="s">
         <v>1093</v>
       </c>
-      <c r="Q267" t="s">
+      <c r="Q267" s="1" t="s">
         <v>1094</v>
       </c>
     </row>
@@ -16688,7 +16692,7 @@
       <c r="P268" t="s">
         <v>1093</v>
       </c>
-      <c r="Q268" t="s">
+      <c r="Q268" s="1" t="s">
         <v>1094</v>
       </c>
     </row>
@@ -16738,7 +16742,7 @@
       <c r="P269" t="s">
         <v>1125</v>
       </c>
-      <c r="Q269" t="s">
+      <c r="Q269" s="1" t="s">
         <v>1126</v>
       </c>
     </row>
@@ -16788,7 +16792,7 @@
       <c r="P270" t="s">
         <v>1115</v>
       </c>
-      <c r="Q270" t="s">
+      <c r="Q270" s="1" t="s">
         <v>1116</v>
       </c>
     </row>
@@ -16838,7 +16842,7 @@
       <c r="P271" t="s">
         <v>1115</v>
       </c>
-      <c r="Q271" t="s">
+      <c r="Q271" s="1" t="s">
         <v>1116</v>
       </c>
     </row>
@@ -16882,7 +16886,7 @@
       <c r="P272" t="s">
         <v>1088</v>
       </c>
-      <c r="Q272" t="s">
+      <c r="Q272" s="1" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -16932,7 +16936,7 @@
       <c r="P273" t="s">
         <v>1088</v>
       </c>
-      <c r="Q273" t="s">
+      <c r="Q273" s="1" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -16982,7 +16986,7 @@
       <c r="P274" t="s">
         <v>1088</v>
       </c>
-      <c r="Q274" t="s">
+      <c r="Q274" s="1" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -17032,7 +17036,7 @@
       <c r="P275" t="s">
         <v>1129</v>
       </c>
-      <c r="Q275" t="s">
+      <c r="Q275" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
@@ -17082,7 +17086,7 @@
       <c r="P276" t="s">
         <v>1146</v>
       </c>
-      <c r="Q276" t="s">
+      <c r="Q276" s="1" t="s">
         <v>1147</v>
       </c>
     </row>
@@ -17129,7 +17133,7 @@
       <c r="P277" t="s">
         <v>1146</v>
       </c>
-      <c r="Q277" t="s">
+      <c r="Q277" s="1" t="s">
         <v>1147</v>
       </c>
     </row>
@@ -17179,7 +17183,7 @@
       <c r="P278" t="s">
         <v>1151</v>
       </c>
-      <c r="Q278" t="s">
+      <c r="Q278" s="1" t="s">
         <v>1152</v>
       </c>
     </row>
@@ -17226,7 +17230,7 @@
       <c r="P279" t="s">
         <v>1158</v>
       </c>
-      <c r="Q279" t="s">
+      <c r="Q279" s="1" t="s">
         <v>1159</v>
       </c>
     </row>
@@ -17276,7 +17280,7 @@
       <c r="P280" t="s">
         <v>1158</v>
       </c>
-      <c r="Q280" t="s">
+      <c r="Q280" s="1" t="s">
         <v>1159</v>
       </c>
     </row>
@@ -17326,7 +17330,7 @@
       <c r="P281" t="s">
         <v>1192</v>
       </c>
-      <c r="Q281" t="s">
+      <c r="Q281" s="1" t="s">
         <v>1193</v>
       </c>
     </row>
@@ -17370,7 +17374,7 @@
       <c r="P282" t="s">
         <v>1181</v>
       </c>
-      <c r="Q282" t="s">
+      <c r="Q282" s="1" t="s">
         <v>1182</v>
       </c>
     </row>
@@ -17420,7 +17424,7 @@
       <c r="P283" t="s">
         <v>1181</v>
       </c>
-      <c r="Q283" t="s">
+      <c r="Q283" s="1" t="s">
         <v>1182</v>
       </c>
     </row>
@@ -17461,7 +17465,7 @@
       <c r="P284" t="s">
         <v>1164</v>
       </c>
-      <c r="Q284" t="s">
+      <c r="Q284" s="1" t="s">
         <v>1165</v>
       </c>
     </row>
@@ -17505,7 +17509,7 @@
       <c r="P285" t="s">
         <v>1154</v>
       </c>
-      <c r="Q285" t="s">
+      <c r="Q285" s="1" t="s">
         <v>1155</v>
       </c>
     </row>
@@ -17549,7 +17553,7 @@
       <c r="P286" t="s">
         <v>1175</v>
       </c>
-      <c r="Q286" t="s">
+      <c r="Q286" s="1" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -17593,7 +17597,7 @@
       <c r="P287" t="s">
         <v>1175</v>
       </c>
-      <c r="Q287" t="s">
+      <c r="Q287" s="1" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -17643,7 +17647,7 @@
       <c r="P288" t="s">
         <v>1175</v>
       </c>
-      <c r="Q288" t="s">
+      <c r="Q288" s="1" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -17690,7 +17694,7 @@
       <c r="P289" t="s">
         <v>1175</v>
       </c>
-      <c r="Q289" t="s">
+      <c r="Q289" s="1" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -17737,7 +17741,7 @@
       <c r="P290" t="s">
         <v>1175</v>
       </c>
-      <c r="Q290" t="s">
+      <c r="Q290" s="1" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -17787,7 +17791,7 @@
       <c r="P291" t="s">
         <v>1196</v>
       </c>
-      <c r="Q291" t="s">
+      <c r="Q291" s="1" t="s">
         <v>1197</v>
       </c>
     </row>
@@ -17837,7 +17841,7 @@
       <c r="P292" t="s">
         <v>1188</v>
       </c>
-      <c r="Q292" t="s">
+      <c r="Q292" s="1" t="s">
         <v>1189</v>
       </c>
     </row>
@@ -17884,7 +17888,7 @@
       <c r="P293" t="s">
         <v>1161</v>
       </c>
-      <c r="Q293" t="s">
+      <c r="Q293" s="1" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -17934,7 +17938,7 @@
       <c r="P294" t="s">
         <v>1161</v>
       </c>
-      <c r="Q294" t="s">
+      <c r="Q294" s="1" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -17981,7 +17985,7 @@
       <c r="P295" t="s">
         <v>1171</v>
       </c>
-      <c r="Q295" t="s">
+      <c r="Q295" s="1" t="s">
         <v>1172</v>
       </c>
     </row>
@@ -18025,7 +18029,7 @@
       <c r="P296" t="s">
         <v>1178</v>
       </c>
-      <c r="Q296" t="s">
+      <c r="Q296" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -18069,7 +18073,7 @@
       <c r="P297" t="s">
         <v>1178</v>
       </c>
-      <c r="Q297" t="s">
+      <c r="Q297" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -18119,7 +18123,7 @@
       <c r="P298" t="s">
         <v>1178</v>
       </c>
-      <c r="Q298" t="s">
+      <c r="Q298" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -18166,7 +18170,7 @@
       <c r="P299" t="s">
         <v>1178</v>
       </c>
-      <c r="Q299" t="s">
+      <c r="Q299" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -18213,7 +18217,7 @@
       <c r="P300" t="s">
         <v>1178</v>
       </c>
-      <c r="Q300" t="s">
+      <c r="Q300" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -18263,7 +18267,7 @@
       <c r="P301" t="s">
         <v>1199</v>
       </c>
-      <c r="Q301" t="s">
+      <c r="Q301" s="1" t="s">
         <v>1200</v>
       </c>
     </row>
@@ -18313,7 +18317,7 @@
       <c r="P302" t="s">
         <v>1207</v>
       </c>
-      <c r="Q302" t="s">
+      <c r="Q302" s="1" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -18354,7 +18358,7 @@
       <c r="P303" t="s">
         <v>1210</v>
       </c>
-      <c r="Q303" t="s">
+      <c r="Q303" s="1" t="s">
         <v>1211</v>
       </c>
     </row>
@@ -18404,7 +18408,7 @@
       <c r="P304" t="s">
         <v>1215</v>
       </c>
-      <c r="Q304" t="s">
+      <c r="Q304" s="1" t="s">
         <v>1216</v>
       </c>
     </row>
@@ -18451,7 +18455,7 @@
       <c r="P305" t="s">
         <v>1204</v>
       </c>
-      <c r="Q305" t="s">
+      <c r="Q305" s="1" t="s">
         <v>1205</v>
       </c>
     </row>
@@ -18501,7 +18505,7 @@
       <c r="P306" t="s">
         <v>1204</v>
       </c>
-      <c r="Q306" t="s">
+      <c r="Q306" s="1" t="s">
         <v>1205</v>
       </c>
     </row>
@@ -18551,7 +18555,7 @@
       <c r="P307" t="s">
         <v>1220</v>
       </c>
-      <c r="Q307" t="s">
+      <c r="Q307" s="1" t="s">
         <v>1221</v>
       </c>
     </row>
@@ -18601,7 +18605,7 @@
       <c r="P308" t="s">
         <v>1220</v>
       </c>
-      <c r="Q308" t="s">
+      <c r="Q308" s="1" t="s">
         <v>1221</v>
       </c>
     </row>
@@ -18648,7 +18652,7 @@
       <c r="P309" t="s">
         <v>1222</v>
       </c>
-      <c r="Q309" t="s">
+      <c r="Q309" s="1" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18692,7 +18696,7 @@
       <c r="P310" t="s">
         <v>1226</v>
       </c>
-      <c r="Q310" t="s">
+      <c r="Q310" s="1" t="s">
         <v>1227</v>
       </c>
     </row>
@@ -18736,7 +18740,7 @@
       <c r="P311" t="s">
         <v>1230</v>
       </c>
-      <c r="Q311" t="s">
+      <c r="Q311" s="1" t="s">
         <v>1231</v>
       </c>
     </row>

</xml_diff>